<commit_message>
update 11/06/21 before meeting
</commit_message>
<xml_diff>
--- a/refs_jorge_june/Saavedra_Garcia_automobile_gas_generator_v2.xlsx
+++ b/refs_jorge_june/Saavedra_Garcia_automobile_gas_generator_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A489ACE-FE61-48A9-87AC-5329E9E9070B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E22300-A331-440B-888B-6EC6ADA5985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4185,6 +4185,72 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4192,9 +4258,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4221,67 +4284,19 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4296,61 +4311,25 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4365,7 +4344,28 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -25484,8 +25484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AQ217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25526,27 +25526,27 @@
       <c r="B1" s="246"/>
       <c r="C1" s="247"/>
       <c r="D1" s="78"/>
-      <c r="E1" s="267" t="s">
+      <c r="E1" s="272" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="I1" s="267" t="s">
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="I1" s="272" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="M1" s="268" t="s">
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="M1" s="263" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="268"/>
-      <c r="Q1" s="268"/>
-      <c r="R1" s="268"/>
-      <c r="S1" s="268"/>
-      <c r="T1" s="268"/>
-      <c r="U1" s="268"/>
+      <c r="N1" s="263"/>
+      <c r="O1" s="263"/>
+      <c r="P1" s="263"/>
+      <c r="Q1" s="263"/>
+      <c r="R1" s="263"/>
+      <c r="S1" s="263"/>
+      <c r="T1" s="263"/>
+      <c r="U1" s="263"/>
       <c r="V1" s="79"/>
       <c r="W1" s="79"/>
     </row>
@@ -25927,11 +25927,11 @@
       <c r="AQ7" s="35"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A8" s="255" t="s">
+      <c r="A8" s="276" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
+      <c r="B8" s="276"/>
+      <c r="C8" s="276"/>
       <c r="D8" s="78"/>
       <c r="F8" t="s">
         <v>370</v>
@@ -26353,31 +26353,31 @@
       <c r="B17" s="36"/>
       <c r="C17" s="2"/>
       <c r="D17" s="32"/>
-      <c r="F17" s="251" t="s">
+      <c r="F17" s="273" t="s">
         <v>237</v>
       </c>
-      <c r="G17" s="251"/>
-      <c r="H17" s="251"/>
-      <c r="J17" s="252" t="s">
+      <c r="G17" s="273"/>
+      <c r="H17" s="273"/>
+      <c r="J17" s="274" t="s">
         <v>239</v>
       </c>
-      <c r="K17" s="252"/>
-      <c r="L17" s="252"/>
-      <c r="N17" s="253" t="s">
+      <c r="K17" s="274"/>
+      <c r="L17" s="274"/>
+      <c r="N17" s="275" t="s">
         <v>253</v>
       </c>
-      <c r="O17" s="253"/>
-      <c r="P17" s="253"/>
-      <c r="R17" s="265" t="s">
+      <c r="O17" s="275"/>
+      <c r="P17" s="275"/>
+      <c r="R17" s="270" t="s">
         <v>242</v>
       </c>
-      <c r="S17" s="265"/>
-      <c r="T17" s="265"/>
-      <c r="V17" s="266" t="s">
+      <c r="S17" s="270"/>
+      <c r="T17" s="270"/>
+      <c r="V17" s="271" t="s">
         <v>243</v>
       </c>
-      <c r="W17" s="266"/>
-      <c r="X17" s="266"/>
+      <c r="W17" s="271"/>
+      <c r="X17" s="271"/>
       <c r="AA17" s="32"/>
       <c r="AB17" s="32"/>
       <c r="AC17" s="32"/>
@@ -26396,11 +26396,11 @@
       <c r="AP17" s="32"/>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="256" t="s">
+      <c r="A18" s="277" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="256"/>
-      <c r="C18" s="256"/>
+      <c r="B18" s="277"/>
+      <c r="C18" s="277"/>
       <c r="D18" s="78"/>
       <c r="F18" s="10" t="s">
         <v>7</v>
@@ -26654,11 +26654,11 @@
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="257" t="s">
+      <c r="A22" s="278" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="257"/>
-      <c r="C22" s="257"/>
+      <c r="B22" s="278"/>
+      <c r="C22" s="278"/>
       <c r="D22" s="78"/>
       <c r="F22" s="9" t="s">
         <v>212</v>
@@ -26933,11 +26933,11 @@
       <c r="X26" s="8"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="257" t="s">
+      <c r="A27" s="278" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="257"/>
-      <c r="C27" s="257"/>
+      <c r="B27" s="278"/>
+      <c r="C27" s="278"/>
       <c r="D27" s="78"/>
       <c r="F27" s="9" t="str">
         <f t="shared" ref="F27:H30" si="0">E99</f>
@@ -27264,11 +27264,11 @@
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="254" t="s">
+      <c r="A32" s="269" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="254"/>
-      <c r="C32" s="254"/>
+      <c r="B32" s="269"/>
+      <c r="C32" s="269"/>
       <c r="D32" s="78"/>
       <c r="E32" s="71"/>
       <c r="J32" s="9" t="s">
@@ -27361,11 +27361,11 @@
       <c r="P34" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="R34" s="269" t="s">
+      <c r="R34" s="264" t="s">
         <v>698</v>
       </c>
-      <c r="S34" s="270"/>
-      <c r="T34" s="271"/>
+      <c r="S34" s="265"/>
+      <c r="T34" s="266"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -27771,11 +27771,11 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="254" t="s">
+      <c r="A45" s="269" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="254"/>
-      <c r="C45" s="254"/>
+      <c r="B45" s="269"/>
+      <c r="C45" s="269"/>
       <c r="D45" s="78"/>
       <c r="J45" s="9" t="s">
         <v>147</v>
@@ -27883,11 +27883,11 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="258" t="s">
+      <c r="A48" s="279" t="s">
         <v>305</v>
       </c>
-      <c r="B48" s="259"/>
-      <c r="C48" s="260"/>
+      <c r="B48" s="280"/>
+      <c r="C48" s="281"/>
       <c r="D48" s="78"/>
       <c r="J48" s="9"/>
       <c r="K48" s="34"/>
@@ -28194,11 +28194,11 @@
       <c r="P57" s="5"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="261" t="s">
+      <c r="A58" s="282" t="s">
         <v>317</v>
       </c>
-      <c r="B58" s="261"/>
-      <c r="C58" s="261"/>
+      <c r="B58" s="282"/>
+      <c r="C58" s="282"/>
       <c r="N58" s="9" t="s">
         <v>520</v>
       </c>
@@ -28242,11 +28242,11 @@
       <c r="P60" s="5"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="262" t="s">
+      <c r="A61" s="283" t="s">
         <v>319</v>
       </c>
-      <c r="B61" s="262"/>
-      <c r="C61" s="262"/>
+      <c r="B61" s="283"/>
+      <c r="C61" s="283"/>
       <c r="N61" s="9" t="s">
         <v>613</v>
       </c>
@@ -28257,11 +28257,11 @@
       <c r="P61" s="5"/>
     </row>
     <row r="62" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="263" t="s">
+      <c r="A62" s="257" t="s">
         <v>299</v>
       </c>
-      <c r="B62" s="263"/>
-      <c r="C62" s="264"/>
+      <c r="B62" s="257"/>
+      <c r="C62" s="258"/>
       <c r="E62" t="s">
         <v>144</v>
       </c>
@@ -28299,11 +28299,11 @@
         <f>B70*B79*B126</f>
         <v>0.7774823082743787</v>
       </c>
-      <c r="M63" s="272" t="s">
+      <c r="M63" s="267" t="s">
         <v>302</v>
       </c>
-      <c r="N63" s="272"/>
-      <c r="O63" s="272"/>
+      <c r="N63" s="267"/>
+      <c r="O63" s="267"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -28320,11 +28320,11 @@
         <f>B40*(B19/B41)^U2</f>
         <v>1022.3999406809887</v>
       </c>
-      <c r="M64" s="273" t="s">
+      <c r="M64" s="268" t="s">
         <v>779</v>
       </c>
-      <c r="N64" s="273"/>
-      <c r="O64" s="273"/>
+      <c r="N64" s="268"/>
+      <c r="O64" s="268"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
@@ -28454,11 +28454,11 @@
         <v>114</v>
       </c>
       <c r="D71" s="78"/>
-      <c r="M71" s="273" t="s">
+      <c r="M71" s="268" t="s">
         <v>303</v>
       </c>
-      <c r="N71" s="273"/>
-      <c r="O71" s="273"/>
+      <c r="N71" s="268"/>
+      <c r="O71" s="268"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="53" t="s">
@@ -28558,11 +28558,11 @@
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="254" t="s">
+      <c r="A78" s="269" t="s">
         <v>135</v>
       </c>
-      <c r="B78" s="254"/>
-      <c r="C78" s="254"/>
+      <c r="B78" s="269"/>
+      <c r="C78" s="269"/>
       <c r="D78" s="32"/>
       <c r="F78" t="s">
         <v>321</v>
@@ -28691,11 +28691,11 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="254" t="s">
+      <c r="A82" s="269" t="s">
         <v>332</v>
       </c>
-      <c r="B82" s="254"/>
-      <c r="C82" s="254"/>
+      <c r="B82" s="269"/>
+      <c r="C82" s="269"/>
       <c r="D82" s="32"/>
       <c r="E82" s="35">
         <f>E81-E80</f>
@@ -28824,11 +28824,11 @@
       <c r="D86" s="78"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="279" t="s">
+      <c r="A87" s="256" t="s">
         <v>300</v>
       </c>
-      <c r="B87" s="263"/>
-      <c r="C87" s="264"/>
+      <c r="B87" s="257"/>
+      <c r="C87" s="258"/>
       <c r="D87" s="32"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -28884,11 +28884,11 @@
       <c r="D91" s="32"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="279" t="s">
+      <c r="A92" s="256" t="s">
         <v>329</v>
       </c>
-      <c r="B92" s="263"/>
-      <c r="C92" s="263"/>
+      <c r="B92" s="257"/>
+      <c r="C92" s="257"/>
       <c r="D92" s="32"/>
       <c r="E92" s="2"/>
     </row>
@@ -28948,17 +28948,17 @@
       <c r="D97" s="32"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="263" t="s">
+      <c r="A98" s="257" t="s">
         <v>180</v>
       </c>
-      <c r="B98" s="263"/>
-      <c r="C98" s="263"/>
+      <c r="B98" s="257"/>
+      <c r="C98" s="257"/>
       <c r="D98" s="32"/>
-      <c r="E98" s="263" t="s">
+      <c r="E98" s="257" t="s">
         <v>469</v>
       </c>
-      <c r="F98" s="263"/>
-      <c r="G98" s="263"/>
+      <c r="F98" s="257"/>
+      <c r="G98" s="257"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
@@ -29179,13 +29179,13 @@
         <v>217</v>
       </c>
       <c r="B111"/>
-      <c r="E111" s="280" t="s">
+      <c r="E111" s="259" t="s">
         <v>218</v>
       </c>
-      <c r="F111" s="280"/>
-      <c r="G111" s="280"/>
-      <c r="H111" s="280"/>
-      <c r="I111" s="280"/>
+      <c r="F111" s="259"/>
+      <c r="G111" s="259"/>
+      <c r="H111" s="259"/>
+      <c r="I111" s="259"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -29334,15 +29334,15 @@
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="281" t="s">
+      <c r="A123" s="260" t="s">
         <v>181</v>
       </c>
-      <c r="B123" s="281"/>
-      <c r="H123" s="268" t="s">
+      <c r="B123" s="260"/>
+      <c r="H123" s="263" t="s">
         <v>487</v>
       </c>
-      <c r="I123" s="268"/>
-      <c r="J123" s="268"/>
+      <c r="I123" s="263"/>
+      <c r="J123" s="263"/>
     </row>
     <row r="124" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
@@ -29353,11 +29353,11 @@
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="32"/>
-      <c r="H124" s="276" t="s">
+      <c r="H124" s="253" t="s">
         <v>488</v>
       </c>
-      <c r="I124" s="276"/>
-      <c r="J124" s="276"/>
+      <c r="I124" s="253"/>
+      <c r="J124" s="253"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
@@ -29618,16 +29618,16 @@
       <c r="D138" s="32"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" s="282" t="s">
+      <c r="A139" s="261" t="s">
         <v>186</v>
       </c>
-      <c r="B139" s="282"/>
+      <c r="B139" s="261"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="283" t="s">
+      <c r="A140" s="262" t="s">
         <v>304</v>
       </c>
-      <c r="B140" s="283"/>
+      <c r="B140" s="262"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
@@ -29666,10 +29666,10 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="274" t="s">
+      <c r="A145" s="251" t="s">
         <v>187</v>
       </c>
-      <c r="B145" s="275"/>
+      <c r="B145" s="252"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
@@ -29708,10 +29708,10 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="277" t="s">
+      <c r="A150" s="254" t="s">
         <v>259</v>
       </c>
-      <c r="B150" s="278"/>
+      <c r="B150" s="255"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="32" t="s">
@@ -29938,10 +29938,10 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="251" t="s">
+      <c r="A168" s="273" t="s">
         <v>339</v>
       </c>
-      <c r="B168" s="251"/>
+      <c r="B168" s="273"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
@@ -30777,28 +30777,6 @@
     <row r="217" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="H124:J124"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="E111:I111"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="H123:J123"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="M63:O63"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="M71:O71"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:U1"/>
     <mergeCell ref="A168:B168"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F17:H17"/>
@@ -30815,6 +30793,28 @@
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A62:C62"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:U1"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="M71:O71"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="H124:J124"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="E111:I111"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="H123:J123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -30866,17 +30866,17 @@
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
-      <c r="F1" s="269" t="s">
+      <c r="F1" s="264" t="s">
         <v>432</v>
       </c>
-      <c r="G1" s="270"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="285" t="s">
+      <c r="G1" s="265"/>
+      <c r="H1" s="266"/>
+      <c r="I1" s="290" t="s">
         <v>422</v>
       </c>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="287"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="292"/>
       <c r="N1" s="108" t="s">
         <v>476</v>
       </c>
@@ -30974,26 +30974,26 @@
         <f>'1D Analysis'!Q2</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="AG3" s="294" t="s">
+      <c r="AG3" s="288" t="s">
         <v>412</v>
       </c>
-      <c r="AH3" s="294"/>
-      <c r="AI3" s="294"/>
-      <c r="AJ3" s="293" t="s">
+      <c r="AH3" s="288"/>
+      <c r="AI3" s="288"/>
+      <c r="AJ3" s="287" t="s">
         <v>413</v>
       </c>
-      <c r="AK3" s="293"/>
-      <c r="AL3" s="293"/>
-      <c r="AM3" s="292" t="s">
+      <c r="AK3" s="287"/>
+      <c r="AL3" s="287"/>
+      <c r="AM3" s="286" t="s">
         <v>414</v>
       </c>
-      <c r="AN3" s="292"/>
-      <c r="AO3" s="292"/>
-      <c r="AP3" s="284" t="s">
+      <c r="AN3" s="286"/>
+      <c r="AO3" s="286"/>
+      <c r="AP3" s="289" t="s">
         <v>415</v>
       </c>
-      <c r="AQ3" s="284"/>
-      <c r="AR3" s="284"/>
+      <c r="AQ3" s="289"/>
+      <c r="AR3" s="289"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
@@ -31890,11 +31890,11 @@
       </c>
     </row>
     <row r="15" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="265" t="s">
+      <c r="A15" s="270" t="s">
         <v>442</v>
       </c>
-      <c r="B15" s="265"/>
-      <c r="C15" s="265"/>
+      <c r="B15" s="270"/>
+      <c r="C15" s="270"/>
       <c r="F15" s="123" t="s">
         <v>275</v>
       </c>
@@ -31955,11 +31955,11 @@
       </c>
     </row>
     <row r="16" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="291" t="s">
+      <c r="A16" s="285" t="s">
         <v>443</v>
       </c>
-      <c r="B16" s="291"/>
-      <c r="C16" s="291"/>
+      <c r="B16" s="285"/>
+      <c r="C16" s="285"/>
       <c r="D16" t="s">
         <v>444</v>
       </c>
@@ -34640,17 +34640,17 @@
       </c>
     </row>
     <row r="52" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="N52" s="289" t="e">
+      <c r="N52" s="293" t="e">
         <f>NISRE!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="O52" s="289"/>
-      <c r="P52" s="289"/>
-      <c r="Q52" s="290" t="s">
+      <c r="O52" s="293"/>
+      <c r="P52" s="293"/>
+      <c r="Q52" s="294" t="s">
         <v>486</v>
       </c>
-      <c r="R52" s="290"/>
-      <c r="S52" s="290"/>
+      <c r="R52" s="294"/>
+      <c r="S52" s="294"/>
       <c r="T52">
         <f>L9</f>
         <v>254.08869342764129</v>
@@ -37509,7 +37509,7 @@
       <c r="AE78" s="73"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" s="288" t="s">
+      <c r="A83" s="284" t="s">
         <v>467</v>
       </c>
       <c r="B83" t="s">
@@ -37517,12 +37517,12 @@
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84" s="288"/>
+      <c r="A84" s="284"/>
       <c r="H84" s="35"/>
       <c r="I84" s="35"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85" s="288"/>
+      <c r="A85" s="284"/>
       <c r="B85" s="40" t="s">
         <v>653</v>
       </c>
@@ -37561,7 +37561,7 @@
       <c r="Q85" s="41"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86" s="288"/>
+      <c r="A86" s="284"/>
       <c r="B86" s="3" t="s">
         <v>159</v>
       </c>
@@ -37620,7 +37620,7 @@
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87" s="288"/>
+      <c r="A87" s="284"/>
       <c r="B87" s="3">
         <v>0</v>
       </c>
@@ -37671,7 +37671,7 @@
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A88" s="288"/>
+      <c r="A88" s="284"/>
       <c r="B88" s="63">
         <f>E26</f>
         <v>766.42539896919243</v>
@@ -37726,7 +37726,7 @@
       </c>
     </row>
     <row r="89" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="288"/>
+      <c r="A89" s="284"/>
       <c r="B89" s="32"/>
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
@@ -37745,7 +37745,7 @@
       <c r="Q89" s="32"/>
     </row>
     <row r="90" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="288"/>
+      <c r="A90" s="284"/>
       <c r="B90" s="55" t="s">
         <v>225</v>
       </c>
@@ -37784,7 +37784,7 @@
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A91" s="288"/>
+      <c r="A91" s="284"/>
       <c r="B91" s="60">
         <v>0</v>
       </c>
@@ -37939,7 +37939,7 @@
       <c r="M98" s="137"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" s="288" t="s">
+      <c r="A100" s="284" t="s">
         <v>507</v>
       </c>
       <c r="B100" t="s">
@@ -37947,12 +37947,12 @@
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A101" s="288"/>
+      <c r="A101" s="284"/>
       <c r="H101" s="35"/>
       <c r="I101" s="35"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A102" s="288"/>
+      <c r="A102" s="284"/>
       <c r="B102" s="40" t="s">
         <v>647</v>
       </c>
@@ -37991,7 +37991,7 @@
       <c r="Q102" s="41"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A103" s="288"/>
+      <c r="A103" s="284"/>
       <c r="B103" s="3" t="s">
         <v>159</v>
       </c>
@@ -38050,7 +38050,7 @@
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A104" s="288"/>
+      <c r="A104" s="284"/>
       <c r="B104" s="3">
         <v>0</v>
       </c>
@@ -38101,7 +38101,7 @@
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A105" s="288"/>
+      <c r="A105" s="284"/>
       <c r="B105" s="63">
         <f>E36</f>
         <v>736.43459771106996</v>
@@ -38156,7 +38156,7 @@
       </c>
     </row>
     <row r="106" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="288"/>
+      <c r="A106" s="284"/>
       <c r="B106" s="32"/>
       <c r="C106" s="32"/>
       <c r="D106" s="32"/>
@@ -38175,7 +38175,7 @@
       <c r="Q106" s="32"/>
     </row>
     <row r="107" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="288"/>
+      <c r="A107" s="284"/>
       <c r="B107" s="55" t="s">
         <v>225</v>
       </c>
@@ -38214,7 +38214,7 @@
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A108" s="288"/>
+      <c r="A108" s="284"/>
       <c r="B108" s="60">
         <v>0</v>
       </c>
@@ -38369,7 +38369,7 @@
       <c r="M115" s="137"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="288" t="s">
+      <c r="A117" s="284" t="s">
         <v>508</v>
       </c>
       <c r="B117" t="s">
@@ -38377,12 +38377,12 @@
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A118" s="288"/>
+      <c r="A118" s="284"/>
       <c r="H118" s="35"/>
       <c r="I118" s="35"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="288"/>
+      <c r="A119" s="284"/>
       <c r="B119" s="40" t="s">
         <v>659</v>
       </c>
@@ -38421,7 +38421,7 @@
       <c r="Q119" s="41"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A120" s="288"/>
+      <c r="A120" s="284"/>
       <c r="B120" s="3" t="s">
         <v>159</v>
       </c>
@@ -38476,7 +38476,7 @@
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="288"/>
+      <c r="A121" s="284"/>
       <c r="B121" s="3">
         <v>0</v>
       </c>
@@ -38529,7 +38529,7 @@
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="288"/>
+      <c r="A122" s="284"/>
       <c r="B122" s="63">
         <f>E46</f>
         <v>709.23797980811491</v>
@@ -38588,7 +38588,7 @@
       </c>
     </row>
     <row r="123" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="288"/>
+      <c r="A123" s="284"/>
       <c r="B123" s="32"/>
       <c r="C123" s="32"/>
       <c r="D123" s="32"/>
@@ -38607,7 +38607,7 @@
       <c r="Q123" s="32"/>
     </row>
     <row r="124" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="288"/>
+      <c r="A124" s="284"/>
       <c r="B124" s="55" t="s">
         <v>225</v>
       </c>
@@ -38646,7 +38646,7 @@
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="288"/>
+      <c r="A125" s="284"/>
       <c r="B125" s="60">
         <v>0</v>
       </c>
@@ -38697,12 +38697,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A117:A125"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="F1:H1"/>
@@ -38710,6 +38704,12 @@
     <mergeCell ref="A100:A108"/>
     <mergeCell ref="N52:P52"/>
     <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="A117:A125"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AG3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38784,17 +38784,17 @@
       </c>
       <c r="AK1" s="11"/>
       <c r="AL1" s="12"/>
-      <c r="AS1" s="269" t="s">
+      <c r="AS1" s="264" t="s">
         <v>432</v>
       </c>
-      <c r="AT1" s="270"/>
-      <c r="AU1" s="271"/>
-      <c r="AV1" s="285" t="s">
+      <c r="AT1" s="265"/>
+      <c r="AU1" s="266"/>
+      <c r="AV1" s="290" t="s">
         <v>422</v>
       </c>
-      <c r="AW1" s="286"/>
-      <c r="AX1" s="286"/>
-      <c r="AY1" s="287"/>
+      <c r="AW1" s="291"/>
+      <c r="AX1" s="291"/>
+      <c r="AY1" s="292"/>
       <c r="BA1" s="108" t="s">
         <v>476</v>
       </c>
@@ -38898,26 +38898,26 @@
       </c>
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
-      <c r="CF3" s="306" t="s">
+      <c r="CF3" s="305" t="s">
         <v>412</v>
       </c>
-      <c r="CG3" s="306"/>
-      <c r="CH3" s="306"/>
-      <c r="CI3" s="293" t="s">
+      <c r="CG3" s="305"/>
+      <c r="CH3" s="305"/>
+      <c r="CI3" s="287" t="s">
         <v>413</v>
       </c>
-      <c r="CJ3" s="293"/>
-      <c r="CK3" s="293"/>
-      <c r="CL3" s="292" t="s">
+      <c r="CJ3" s="287"/>
+      <c r="CK3" s="287"/>
+      <c r="CL3" s="286" t="s">
         <v>414</v>
       </c>
-      <c r="CM3" s="292"/>
-      <c r="CN3" s="292"/>
-      <c r="CO3" s="305" t="s">
+      <c r="CM3" s="286"/>
+      <c r="CN3" s="286"/>
+      <c r="CO3" s="304" t="s">
         <v>415</v>
       </c>
-      <c r="CP3" s="305"/>
-      <c r="CQ3" s="305"/>
+      <c r="CP3" s="304"/>
+      <c r="CQ3" s="304"/>
     </row>
     <row r="4" spans="36:95" x14ac:dyDescent="0.25">
       <c r="AJ4" s="9" t="str">
@@ -39810,11 +39810,11 @@
       <c r="CQ14" s="112"/>
     </row>
     <row r="15" spans="36:95" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="265" t="s">
+      <c r="AJ15" s="270" t="s">
         <v>442</v>
       </c>
-      <c r="AK15" s="265"/>
-      <c r="AL15" s="265"/>
+      <c r="AK15" s="270"/>
+      <c r="AL15" s="270"/>
       <c r="AP15" s="3" t="s">
         <v>35</v>
       </c>
@@ -39879,11 +39879,11 @@
       <c r="CQ15" s="112"/>
     </row>
     <row r="16" spans="36:95" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="291" t="s">
+      <c r="AJ16" s="285" t="s">
         <v>443</v>
       </c>
-      <c r="AK16" s="291"/>
-      <c r="AL16" s="291"/>
+      <c r="AK16" s="285"/>
+      <c r="AL16" s="285"/>
       <c r="AM16" t="s">
         <v>444</v>
       </c>
@@ -40417,17 +40417,17 @@
       <c r="F25" t="s">
         <v>588</v>
       </c>
-      <c r="G25" s="307" t="s">
+      <c r="G25" s="300" t="s">
         <v>585</v>
       </c>
-      <c r="H25" s="308"/>
-      <c r="I25" s="308"/>
-      <c r="J25" s="308"/>
-      <c r="K25" s="308"/>
-      <c r="Y25" s="291" t="s">
+      <c r="H25" s="301"/>
+      <c r="I25" s="301"/>
+      <c r="J25" s="301"/>
+      <c r="K25" s="301"/>
+      <c r="Y25" s="285" t="s">
         <v>628</v>
       </c>
-      <c r="Z25" s="291"/>
+      <c r="Z25" s="285"/>
       <c r="AA25" s="1" t="s">
         <v>72</v>
       </c>
@@ -40634,10 +40634,10 @@
       <c r="DC25" s="73"/>
     </row>
     <row r="26" spans="1:133" x14ac:dyDescent="0.25">
-      <c r="A26" s="299" t="s">
+      <c r="A26" s="308" t="s">
         <v>532</v>
       </c>
-      <c r="B26" s="300"/>
+      <c r="B26" s="309"/>
       <c r="C26" s="186"/>
       <c r="D26" s="186"/>
       <c r="E26" s="146"/>
@@ -40665,18 +40665,18 @@
         <f>(J26+J27)/2*(G27-G26)</f>
         <v>3.7968749999997302E-3</v>
       </c>
-      <c r="AA26" s="302" t="s">
+      <c r="AA26" s="310" t="s">
         <v>757</v>
       </c>
-      <c r="AB26" s="303"/>
-      <c r="AC26" s="302" t="s">
+      <c r="AB26" s="311"/>
+      <c r="AC26" s="310" t="s">
         <v>758</v>
       </c>
-      <c r="AD26" s="303"/>
-      <c r="AE26" s="302" t="s">
+      <c r="AD26" s="311"/>
+      <c r="AE26" s="310" t="s">
         <v>759</v>
       </c>
-      <c r="AF26" s="303"/>
+      <c r="AF26" s="311"/>
       <c r="AG26" s="146"/>
       <c r="AH26" s="146"/>
       <c r="AJ26" s="201" t="s">
@@ -41996,10 +41996,10 @@
         <f t="shared" si="31"/>
         <v>1.2656249999998205E-3</v>
       </c>
-      <c r="Y31" s="291" t="s">
+      <c r="Y31" s="285" t="s">
         <v>569</v>
       </c>
-      <c r="Z31" s="304"/>
+      <c r="Z31" s="297"/>
       <c r="AA31" s="165" t="s">
         <v>526</v>
       </c>
@@ -42853,10 +42853,10 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="Y34" s="291" t="s">
+      <c r="Y34" s="285" t="s">
         <v>569</v>
       </c>
-      <c r="Z34" s="291"/>
+      <c r="Z34" s="285"/>
       <c r="AA34" s="166" t="s">
         <v>590</v>
       </c>
@@ -43441,10 +43441,10 @@
       <c r="V36" s="73"/>
       <c r="W36" s="73"/>
       <c r="X36" s="73"/>
-      <c r="Y36" s="291" t="s">
+      <c r="Y36" s="285" t="s">
         <v>562</v>
       </c>
-      <c r="Z36" s="304"/>
+      <c r="Z36" s="297"/>
       <c r="AA36" s="165" t="s">
         <v>556</v>
       </c>
@@ -43742,10 +43742,10 @@
         <f t="shared" ref="K37" si="54">(J37+J36)/2*(G37-G36)*SUM($I$36:$I$46)</f>
         <v>0</v>
       </c>
-      <c r="Y37" s="291" t="s">
+      <c r="Y37" s="285" t="s">
         <v>568</v>
       </c>
-      <c r="Z37" s="304"/>
+      <c r="Z37" s="297"/>
       <c r="AA37" s="166" t="s">
         <v>557</v>
       </c>
@@ -44008,10 +44008,10 @@
       <c r="EC37" s="73"/>
     </row>
     <row r="38" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="299" t="s">
+      <c r="A38" s="308" t="s">
         <v>533</v>
       </c>
-      <c r="B38" s="300"/>
+      <c r="B38" s="309"/>
       <c r="C38" s="186"/>
       <c r="D38" s="186"/>
       <c r="E38" s="146"/>
@@ -44039,10 +44039,10 @@
         <f t="shared" ref="K38:K45" si="62">(J38+J37)/2*(G38-G37)</f>
         <v>0</v>
       </c>
-      <c r="Y38" s="291" t="s">
+      <c r="Y38" s="285" t="s">
         <v>563</v>
       </c>
-      <c r="Z38" s="304"/>
+      <c r="Z38" s="297"/>
       <c r="AA38" s="168" t="s">
         <v>561</v>
       </c>
@@ -44308,10 +44308,10 @@
         <f t="shared" si="62"/>
         <v>2.5312499999996171E-4</v>
       </c>
-      <c r="Y39" s="291" t="s">
+      <c r="Y39" s="285" t="s">
         <v>565</v>
       </c>
-      <c r="Z39" s="304"/>
+      <c r="Z39" s="297"/>
       <c r="AA39" s="165" t="s">
         <v>567</v>
       </c>
@@ -44334,10 +44334,10 @@
         <v>8.5565759378543174E-2</v>
       </c>
       <c r="AG39" s="202"/>
-      <c r="AH39" s="301" t="s">
+      <c r="AH39" s="295" t="s">
         <v>760</v>
       </c>
-      <c r="AI39" s="301"/>
+      <c r="AI39" s="295"/>
       <c r="AJ39" s="73"/>
       <c r="AK39">
         <v>14</v>
@@ -44603,8 +44603,8 @@
         <v>1.8</v>
       </c>
       <c r="AG40" s="2"/>
-      <c r="AH40" s="301"/>
-      <c r="AI40" s="301"/>
+      <c r="AH40" s="295"/>
+      <c r="AI40" s="295"/>
       <c r="AK40">
         <v>15</v>
       </c>
@@ -45393,10 +45393,10 @@
         <f t="shared" si="62"/>
         <v>2.2781249999997261E-3</v>
       </c>
-      <c r="Y43" s="291" t="s">
+      <c r="Y43" s="285" t="s">
         <v>564</v>
       </c>
-      <c r="Z43" s="304"/>
+      <c r="Z43" s="297"/>
       <c r="AA43" s="165" t="s">
         <v>560</v>
       </c>
@@ -46564,11 +46564,11 @@
       <c r="BY54" s="73"/>
       <c r="BZ54" s="73"/>
       <c r="CA54" s="73"/>
-      <c r="CW54" s="291"/>
-      <c r="CX54" s="291"/>
-      <c r="CY54" s="291"/>
-      <c r="CZ54" s="291"/>
-      <c r="DA54" s="291"/>
+      <c r="CW54" s="285"/>
+      <c r="CX54" s="285"/>
+      <c r="CY54" s="285"/>
+      <c r="CZ54" s="285"/>
+      <c r="DA54" s="285"/>
     </row>
     <row r="55" spans="1:105" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -46590,10 +46590,10 @@
       <c r="V55" t="s">
         <v>761</v>
       </c>
-      <c r="Y55" s="288" t="s">
+      <c r="Y55" s="284" t="s">
         <v>627</v>
       </c>
-      <c r="Z55" s="288"/>
+      <c r="Z55" s="284"/>
       <c r="AA55" s="1" t="s">
         <v>118</v>
       </c>
@@ -46619,10 +46619,10 @@
         <f>AY9</f>
         <v>254.08869342764129</v>
       </c>
-      <c r="BE55" s="253" t="s">
+      <c r="BE55" s="275" t="s">
         <v>622</v>
       </c>
-      <c r="BF55" s="253"/>
+      <c r="BF55" s="275"/>
       <c r="BG55" s="209"/>
       <c r="BH55" s="210" t="s">
         <v>637</v>
@@ -46665,22 +46665,22 @@
       <c r="F56" t="s">
         <v>588</v>
       </c>
-      <c r="G56" s="309" t="s">
+      <c r="G56" s="302" t="s">
         <v>584</v>
       </c>
-      <c r="H56" s="310"/>
-      <c r="I56" s="310"/>
-      <c r="J56" s="310"/>
-      <c r="K56" s="310"/>
-      <c r="R56" s="309" t="s">
+      <c r="H56" s="303"/>
+      <c r="I56" s="303"/>
+      <c r="J56" s="303"/>
+      <c r="K56" s="303"/>
+      <c r="R56" s="302" t="s">
         <v>583</v>
       </c>
-      <c r="S56" s="310"/>
-      <c r="T56" s="310"/>
-      <c r="U56" s="310"/>
-      <c r="V56" s="310"/>
-      <c r="Y56" s="288"/>
-      <c r="Z56" s="288"/>
+      <c r="S56" s="303"/>
+      <c r="T56" s="303"/>
+      <c r="U56" s="303"/>
+      <c r="V56" s="303"/>
+      <c r="Y56" s="284"/>
+      <c r="Z56" s="284"/>
       <c r="AA56" s="1" t="s">
         <v>73</v>
       </c>
@@ -46920,10 +46920,10 @@
         <f>(J57+J58)/2*(G58-G57)</f>
         <v>9.5809999999988179E-3</v>
       </c>
-      <c r="N57" s="295" t="s">
+      <c r="N57" s="306" t="s">
         <v>764</v>
       </c>
-      <c r="O57" s="296"/>
+      <c r="O57" s="307"/>
       <c r="R57" s="171">
         <f>AL57</f>
         <v>0.10590399514291465</v>
@@ -46938,18 +46938,18 @@
         <f>V58</f>
         <v>0</v>
       </c>
-      <c r="AA57" s="297" t="s">
+      <c r="AA57" s="298" t="s">
         <v>757</v>
       </c>
-      <c r="AB57" s="298"/>
-      <c r="AC57" s="297" t="s">
+      <c r="AB57" s="299"/>
+      <c r="AC57" s="298" t="s">
         <v>758</v>
       </c>
-      <c r="AD57" s="298"/>
-      <c r="AE57" s="297" t="s">
+      <c r="AD57" s="299"/>
+      <c r="AE57" s="298" t="s">
         <v>759</v>
       </c>
-      <c r="AF57" s="298"/>
+      <c r="AF57" s="299"/>
       <c r="AG57" s="204"/>
       <c r="AH57" s="204"/>
       <c r="AJ57" s="201" t="s">
@@ -48555,10 +48555,10 @@
         <f t="shared" si="115"/>
         <v>0</v>
       </c>
-      <c r="Y62" s="291" t="s">
+      <c r="Y62" s="285" t="s">
         <v>569</v>
       </c>
-      <c r="Z62" s="311"/>
+      <c r="Z62" s="296"/>
       <c r="AA62" s="165" t="s">
         <v>526</v>
       </c>
@@ -49507,11 +49507,11 @@
         <f t="shared" si="132"/>
         <v>0</v>
       </c>
-      <c r="X65" s="291" t="s">
+      <c r="X65" s="285" t="s">
         <v>569</v>
       </c>
-      <c r="Y65" s="291"/>
-      <c r="Z65" s="311"/>
+      <c r="Y65" s="285"/>
+      <c r="Z65" s="296"/>
       <c r="AA65" s="166" t="s">
         <v>590</v>
       </c>
@@ -50164,10 +50164,10 @@
       </c>
       <c r="W67" s="73"/>
       <c r="X67"/>
-      <c r="Y67" s="291" t="s">
+      <c r="Y67" s="285" t="s">
         <v>562</v>
       </c>
-      <c r="Z67" s="311"/>
+      <c r="Z67" s="296"/>
       <c r="AA67" s="165" t="s">
         <v>556</v>
       </c>
@@ -50530,10 +50530,10 @@
         <v>0</v>
       </c>
       <c r="X68" s="73"/>
-      <c r="Y68" s="291" t="s">
+      <c r="Y68" s="285" t="s">
         <v>568</v>
       </c>
-      <c r="Z68" s="311"/>
+      <c r="Z68" s="296"/>
       <c r="AA68" s="166" t="s">
         <v>557</v>
       </c>
@@ -50868,11 +50868,11 @@
         <f t="shared" si="132"/>
         <v>0</v>
       </c>
-      <c r="X69" s="291" t="s">
+      <c r="X69" s="285" t="s">
         <v>563</v>
       </c>
-      <c r="Y69" s="291"/>
-      <c r="Z69" s="311"/>
+      <c r="Y69" s="285"/>
+      <c r="Z69" s="296"/>
       <c r="AA69" s="165" t="s">
         <v>561</v>
       </c>
@@ -51195,11 +51195,11 @@
         <f t="shared" si="132"/>
         <v>3.1832167890308237E-3</v>
       </c>
-      <c r="X70" s="291" t="s">
+      <c r="X70" s="285" t="s">
         <v>565</v>
       </c>
-      <c r="Y70" s="291"/>
-      <c r="Z70" s="311"/>
+      <c r="Y70" s="285"/>
+      <c r="Z70" s="296"/>
       <c r="AA70" s="165" t="s">
         <v>567</v>
       </c>
@@ -51222,10 +51222,10 @@
         <v>9.1612651514654961E-2</v>
       </c>
       <c r="AG70" s="202"/>
-      <c r="AH70" s="301" t="s">
+      <c r="AH70" s="295" t="s">
         <v>760</v>
       </c>
-      <c r="AI70" s="301"/>
+      <c r="AI70" s="295"/>
       <c r="AK70">
         <v>14</v>
       </c>
@@ -51556,8 +51556,8 @@
         <v>118.56742054402559</v>
       </c>
       <c r="AG71" s="2"/>
-      <c r="AH71" s="301"/>
-      <c r="AI71" s="301"/>
+      <c r="AH71" s="295"/>
+      <c r="AI71" s="295"/>
       <c r="AJ71" s="73"/>
       <c r="AK71">
         <v>15</v>
@@ -51866,11 +51866,11 @@
         <f t="shared" si="132"/>
         <v>1.5916083945154608E-2</v>
       </c>
-      <c r="X72" s="291" t="s">
+      <c r="X72" s="285" t="s">
         <v>566</v>
       </c>
-      <c r="Y72" s="291"/>
-      <c r="Z72" s="311"/>
+      <c r="Y72" s="285"/>
+      <c r="Z72" s="296"/>
       <c r="AA72" s="165" t="s">
         <v>558</v>
       </c>
@@ -52199,11 +52199,11 @@
         <v>2.2282517523216014E-2</v>
       </c>
       <c r="W73" s="136"/>
-      <c r="X73" s="291" t="s">
+      <c r="X73" s="285" t="s">
         <v>564</v>
       </c>
-      <c r="Y73" s="291"/>
-      <c r="Z73" s="311"/>
+      <c r="Y73" s="285"/>
+      <c r="Z73" s="296"/>
       <c r="AA73" s="165" t="s">
         <v>559</v>
       </c>
@@ -53966,7 +53966,7 @@
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="U86" s="224"/>
-      <c r="AJ86" s="288" t="s">
+      <c r="AJ86" s="284" t="s">
         <v>467</v>
       </c>
       <c r="AK86" t="s">
@@ -53984,7 +53984,7 @@
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="U87" s="224"/>
-      <c r="AJ87" s="288"/>
+      <c r="AJ87" s="284"/>
       <c r="AU87" s="35"/>
       <c r="AV87" s="35"/>
       <c r="BH87" s="32"/>
@@ -53999,7 +53999,7 @@
         <f>B85/AK23</f>
         <v>6.9999999999999938</v>
       </c>
-      <c r="AJ88" s="288"/>
+      <c r="AJ88" s="284"/>
       <c r="AK88" s="40" t="s">
         <v>666</v>
       </c>
@@ -54056,7 +54056,7 @@
       </c>
     </row>
     <row r="89" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="288"/>
+      <c r="AJ89" s="284"/>
       <c r="AK89" s="3" t="s">
         <v>159</v>
       </c>
@@ -54133,7 +54133,7 @@
       </c>
     </row>
     <row r="90" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="288"/>
+      <c r="AJ90" s="284"/>
       <c r="AK90" s="3">
         <v>0</v>
       </c>
@@ -54194,7 +54194,7 @@
       <c r="BU90" s="32"/>
     </row>
     <row r="91" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="288"/>
+      <c r="AJ91" s="284"/>
       <c r="AK91" s="63">
         <f>AN26</f>
         <v>768.22125433469159</v>
@@ -54266,7 +54266,7 @@
       </c>
     </row>
     <row r="92" spans="1:93" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ92" s="288"/>
+      <c r="AJ92" s="284"/>
       <c r="AK92" s="32"/>
       <c r="AL92" s="32"/>
       <c r="AM92" s="32"/>
@@ -54302,7 +54302,7 @@
       </c>
     </row>
     <row r="93" spans="1:93" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ93" s="288"/>
+      <c r="AJ93" s="284"/>
       <c r="AK93" s="55" t="s">
         <v>225</v>
       </c>
@@ -54349,7 +54349,7 @@
       <c r="BU93" s="78"/>
     </row>
     <row r="94" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="288"/>
+      <c r="AJ94" s="284"/>
       <c r="AK94" s="60">
         <v>0</v>
       </c>
@@ -54584,7 +54584,7 @@
       <c r="BU102" s="73"/>
     </row>
     <row r="103" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ103" s="288" t="s">
+      <c r="AJ103" s="284" t="s">
         <v>507</v>
       </c>
       <c r="AK103" t="s">
@@ -54600,7 +54600,7 @@
       <c r="BU103" s="73"/>
     </row>
     <row r="104" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ104" s="288"/>
+      <c r="AJ104" s="284"/>
       <c r="AR104" s="35"/>
       <c r="AS104" s="35"/>
       <c r="BH104" s="32"/>
@@ -54613,7 +54613,7 @@
       <c r="BU104" s="73"/>
     </row>
     <row r="105" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ105" s="288"/>
+      <c r="AJ105" s="284"/>
       <c r="AK105" s="40" t="s">
         <v>671</v>
       </c>
@@ -54660,7 +54660,7 @@
       <c r="BU105" s="32"/>
     </row>
     <row r="106" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ106" s="288"/>
+      <c r="AJ106" s="284"/>
       <c r="AK106" s="3" t="s">
         <v>159</v>
       </c>
@@ -54727,7 +54727,7 @@
       <c r="BU106" s="32"/>
     </row>
     <row r="107" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ107" s="288"/>
+      <c r="AJ107" s="284"/>
       <c r="AK107" s="3">
         <v>0</v>
       </c>
@@ -54788,7 +54788,7 @@
       <c r="BU107" s="32"/>
     </row>
     <row r="108" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ108" s="288"/>
+      <c r="AJ108" s="284"/>
       <c r="AK108" s="63">
         <f>AN36</f>
         <v>736.43459771106996</v>
@@ -54851,7 +54851,7 @@
       <c r="BU108" s="71"/>
     </row>
     <row r="109" spans="36:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ109" s="288"/>
+      <c r="AJ109" s="284"/>
       <c r="AK109" s="32"/>
       <c r="AL109" s="32"/>
       <c r="AM109" s="32"/>
@@ -54878,7 +54878,7 @@
       <c r="BU109" s="32"/>
     </row>
     <row r="110" spans="36:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ110" s="288"/>
+      <c r="AJ110" s="284"/>
       <c r="AK110" s="55" t="s">
         <v>225</v>
       </c>
@@ -54925,7 +54925,7 @@
       <c r="BU110" s="78"/>
     </row>
     <row r="111" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ111" s="288"/>
+      <c r="AJ111" s="284"/>
       <c r="AK111" s="60">
         <v>0</v>
       </c>
@@ -55160,7 +55160,7 @@
       <c r="BU119" s="73"/>
     </row>
     <row r="120" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ120" s="288" t="s">
+      <c r="AJ120" s="284" t="s">
         <v>508</v>
       </c>
       <c r="AK120" t="s">
@@ -55176,7 +55176,7 @@
       <c r="BU120" s="73"/>
     </row>
     <row r="121" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ121" s="288"/>
+      <c r="AJ121" s="284"/>
       <c r="AR121" s="35"/>
       <c r="AS121" s="35"/>
       <c r="BH121" s="32"/>
@@ -55189,7 +55189,7 @@
       <c r="BU121" s="73"/>
     </row>
     <row r="122" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ122" s="288"/>
+      <c r="AJ122" s="284"/>
       <c r="AK122" s="40" t="s">
         <v>677</v>
       </c>
@@ -55236,7 +55236,7 @@
       <c r="BU122" s="32"/>
     </row>
     <row r="123" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ123" s="288"/>
+      <c r="AJ123" s="284"/>
       <c r="AK123" s="3" t="s">
         <v>159</v>
       </c>
@@ -55299,7 +55299,7 @@
       <c r="BU123" s="32"/>
     </row>
     <row r="124" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ124" s="288"/>
+      <c r="AJ124" s="284"/>
       <c r="AK124" s="3">
         <v>0</v>
       </c>
@@ -55360,7 +55360,7 @@
       <c r="BU124" s="32"/>
     </row>
     <row r="125" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ125" s="288"/>
+      <c r="AJ125" s="284"/>
       <c r="AK125" s="63">
         <f>AN46</f>
         <v>707.61315337357701</v>
@@ -55427,7 +55427,7 @@
       <c r="BU125" s="71"/>
     </row>
     <row r="126" spans="36:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ126" s="288"/>
+      <c r="AJ126" s="284"/>
       <c r="AK126" s="32"/>
       <c r="AL126" s="32"/>
       <c r="AM126" s="32"/>
@@ -55454,7 +55454,7 @@
       <c r="BU126" s="32"/>
     </row>
     <row r="127" spans="36:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ127" s="288"/>
+      <c r="AJ127" s="284"/>
       <c r="AK127" s="55" t="s">
         <v>225</v>
       </c>
@@ -55501,7 +55501,7 @@
       <c r="BU127" s="78"/>
     </row>
     <row r="128" spans="36:73" x14ac:dyDescent="0.25">
-      <c r="AJ128" s="288"/>
+      <c r="AJ128" s="284"/>
       <c r="AK128" s="60">
         <v>0</v>
       </c>
@@ -55565,6 +55565,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="CW54:DA54"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="AA57:AB57"/>
+    <mergeCell ref="BE55:BF55"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="AH39:AI40"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="Y39:Z39"/>
+    <mergeCell ref="Y43:Z43"/>
+    <mergeCell ref="CO3:CQ3"/>
+    <mergeCell ref="AS1:AU1"/>
+    <mergeCell ref="AV1:AY1"/>
+    <mergeCell ref="CF3:CH3"/>
+    <mergeCell ref="CI3:CK3"/>
+    <mergeCell ref="CL3:CN3"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="Y37:Z37"/>
+    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="R56:V56"/>
+    <mergeCell ref="AJ120:AJ128"/>
+    <mergeCell ref="AJ15:AL15"/>
+    <mergeCell ref="AJ16:AL16"/>
+    <mergeCell ref="AJ86:AJ94"/>
+    <mergeCell ref="AJ103:AJ111"/>
     <mergeCell ref="AH70:AI71"/>
     <mergeCell ref="X72:Z72"/>
     <mergeCell ref="X73:Z73"/>
@@ -55581,34 +55609,6 @@
     <mergeCell ref="X69:Z69"/>
     <mergeCell ref="X70:Z70"/>
     <mergeCell ref="AE57:AF57"/>
-    <mergeCell ref="AJ120:AJ128"/>
-    <mergeCell ref="AJ15:AL15"/>
-    <mergeCell ref="AJ16:AL16"/>
-    <mergeCell ref="AJ86:AJ94"/>
-    <mergeCell ref="AJ103:AJ111"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="Y37:Z37"/>
-    <mergeCell ref="G56:K56"/>
-    <mergeCell ref="R56:V56"/>
-    <mergeCell ref="CO3:CQ3"/>
-    <mergeCell ref="AS1:AU1"/>
-    <mergeCell ref="AV1:AY1"/>
-    <mergeCell ref="CF3:CH3"/>
-    <mergeCell ref="CI3:CK3"/>
-    <mergeCell ref="CL3:CN3"/>
-    <mergeCell ref="CW54:DA54"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="AA57:AB57"/>
-    <mergeCell ref="BE55:BF55"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="AH39:AI40"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="Y39:Z39"/>
-    <mergeCell ref="Y43:Z43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>